<commit_message>
#bug: URL decode & display 'DETAILS' block
#bug: Lien Externes decode & display 'DETAILS' block when INFO object
charged
</commit_message>
<xml_diff>
--- a/Analytics-panneau.xlsx
+++ b/Analytics-panneau.xlsx
@@ -5131,18 +5131,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C220" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" topLeftCell="J229" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.42578125" customWidth="1"/>
-    <col min="7" max="9" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="15.7109375" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" style="9" customWidth="1"/>
     <col min="12" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>

</xml_diff>